<commit_message>
Change material 14 for teaching plan
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/14 - 数组公式.xlsx
+++ b/Excel动手实验室 - 材料/14 - 数组公式.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\OfficeTraining\Excel动手实验室 - 材料\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18434" windowHeight="8097"/>
   </bookViews>
   <sheets>
     <sheet name="总计" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="最大值" sheetId="3" r:id="rId3"/>
     <sheet name="编辑" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>股票</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -53,103 +48,97 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>年份</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售额</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售额年增长额</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=B3-B2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售额的年平均增长额</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用数组公式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=AVERAGE((B3-B2),(B4-B3),(B5-B4),(B6-B5),(B7-B6))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contoso</t>
+  </si>
+  <si>
+    <t>Fabrikam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tailspin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A. Datum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Northwind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{=B2:F2*B3:F3}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contoso</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>开盘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>收盘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>一天最大收益</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=D2-C2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>总计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>{=SUM(B2:F2*B3:F3)}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>年份</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>销售额</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>销售额年增长额</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>=B3-B2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>销售额的年平均增长额</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用数组公式</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>=AVERAGE((B3-B2),(B4-B3),(B5-B4),(B6-B5),(B7-B6))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>{=AVERAGE(B3:B7-B2:B6)}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contoso</t>
-  </si>
-  <si>
-    <t>Fabrikam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tailspin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A. Datum</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Northwind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>小计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{=B2:F2*B3:F3}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contoso</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>开盘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>收盘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>一天最大收益</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>=D2-C2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{=MAX(D2:D6-C2:C6)}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Google</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>总计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -157,13 +146,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -171,14 +160,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -187,14 +176,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -247,13 +236,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1">
@@ -268,25 +257,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="强调文字颜色 5" xfId="1" builtinId="45"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -556,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,12 +557,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="13.46484375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -582,19 +571,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -652,12 +641,12 @@
       </c>
       <c r="B7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -665,9 +654,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="1"/>
+    </row>
     <row r="11" spans="1:6">
       <c r="F11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -682,23 +674,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.46484375" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -722,7 +714,7 @@
         <v>88688.800000000279</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -762,23 +754,26 @@
       <c r="C7" s="2"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="9"/>
+      <c r="A9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="12"/>
       <c r="C9" s="1"/>
       <c r="E9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="1" t="e">
+        <f t="array" ref="C11">AVERAGE(B3:B7-B2:B5)</f>
+        <v>#N/A</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -797,10 +792,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -808,20 +803,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10">
+        <v>13</v>
+      </c>
+      <c r="B2" s="9">
         <v>42125</v>
       </c>
       <c r="C2" s="3">
@@ -831,14 +826,14 @@
         <v>357.8</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="10">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9">
         <v>42126</v>
       </c>
       <c r="C3" s="3">
@@ -850,9 +845,9 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9">
         <v>42127</v>
       </c>
       <c r="C4" s="3">
@@ -864,9 +859,9 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="10">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9">
         <v>42128</v>
       </c>
       <c r="C5" s="3">
@@ -878,9 +873,9 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="10">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
         <v>42129</v>
       </c>
       <c r="C6" s="3">
@@ -891,14 +886,11 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="9"/>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="1"/>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -914,14 +906,14 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -929,22 +921,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -966,7 +958,7 @@
       <c r="F2" s="2">
         <v>27</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>34</v>
       </c>
     </row>
@@ -989,13 +981,13 @@
       <c r="F3" s="3">
         <v>63.21</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>287.3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="8">
         <f t="array" ref="B5:F5">B2:F2*B3:F3</f>
@@ -1016,7 +1008,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <f t="array" ref="B7">SUM(B2:F2*B3:F3)</f>

</xml_diff>